<commit_message>
Added WRI policies and recession file and fixed bugs in WebAppData and input files
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -40,7 +40,7 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="86">
   <si>
     <t>Sources:</t>
   </si>
@@ -288,6 +288,30 @@
   <si>
     <t>Psgr LDVs, Gasoline (psgr-mi/BTU)</t>
   </si>
+  <si>
+    <t>Hydrogen vs. Gasoline Efficiency</t>
+  </si>
+  <si>
+    <t>gasoline car efficiency</t>
+  </si>
+  <si>
+    <t>hydrogen FCV efficiency</t>
+  </si>
+  <si>
+    <t>distance multiplier for hydrogen vehicles</t>
+  </si>
+  <si>
+    <t>U.S. Department of Energy Hydrogen Program</t>
+  </si>
+  <si>
+    <t>Hydrogen Fuel Cells</t>
+  </si>
+  <si>
+    <t>https://www.californiahydrogen.org/wp-content/uploads/files/doe_fuelcell_factsheet.pdf</t>
+  </si>
+  <si>
+    <t>Hydrogen Efficiency Adjustment</t>
+  </si>
 </sst>
 </file>
 
@@ -300,7 +324,7 @@
     <numFmt numFmtId="165" formatCode="#,##0_)"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="43">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -548,6 +572,14 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -918,7 +950,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="153">
+  <cellStyleXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyProtection="0">
@@ -1173,8 +1205,9 @@
     <xf numFmtId="49" fontId="33" fillId="0" borderId="8">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1202,8 +1235,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="153"/>
   </cellXfs>
-  <cellStyles count="153">
+  <cellStyles count="154">
     <cellStyle name="20% - Accent1 2" xfId="8"/>
     <cellStyle name="20% - Accent2 2" xfId="9"/>
     <cellStyle name="20% - Accent3 2" xfId="10"/>
@@ -1272,6 +1306,7 @@
     <cellStyle name="Hed Top" xfId="69"/>
     <cellStyle name="Hed Top - SECTION" xfId="70"/>
     <cellStyle name="Hed Top_3-new4" xfId="71"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="72"/>
     <cellStyle name="Input 2" xfId="73"/>
     <cellStyle name="Linked Cell 2" xfId="74"/>
@@ -1386,7 +1421,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1651,7 +1685,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1973,7 +2006,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2242,7 +2274,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2760,7 +2791,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3265,7 +3295,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3548,7 +3577,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3846,7 +3874,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4161,7 +4188,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4496,7 +4522,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5610,10 +5635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5676,117 +5701,148 @@
         <v>19</v>
       </c>
     </row>
+    <row r="14" spans="1:2">
+      <c r="B14" s="7"/>
+    </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="1" t="s">
-        <v>1</v>
+      <c r="B15" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="B17" s="5">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" s="23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="19"/>
+    <row r="23" spans="1:2">
+      <c r="A23" s="19"/>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="19" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="19" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="19" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="19" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="19" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="19" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="19" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="19" t="s">
+    <row r="33" spans="1:1">
+      <c r="A33" s="19" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B19" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10352,8 +10408,8 @@
   </sheetPr>
   <dimension ref="A1:AI14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -11318,107 +11374,141 @@
       <c r="A8" t="s">
         <v>55</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8" s="8">
-        <v>0</v>
-      </c>
-      <c r="T8" s="8">
-        <v>0</v>
-      </c>
-      <c r="U8" s="8">
-        <v>0</v>
-      </c>
-      <c r="V8" s="8">
-        <v>0</v>
-      </c>
-      <c r="W8" s="8">
-        <v>0</v>
-      </c>
-      <c r="X8" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="8">
-        <v>0</v>
+      <c r="B8" s="4">
+        <f>B4*'Other Values'!$B$31</f>
+        <v>3.8579698245238621E-3</v>
+      </c>
+      <c r="C8" s="4">
+        <f>C4*'Other Values'!$B$31</f>
+        <v>3.8579698245238621E-3</v>
+      </c>
+      <c r="D8" s="4">
+        <f>D4*'Other Values'!$B$31</f>
+        <v>3.8579698245238621E-3</v>
+      </c>
+      <c r="E8" s="4">
+        <f>E4*'Other Values'!$B$31</f>
+        <v>3.8579698245238621E-3</v>
+      </c>
+      <c r="F8" s="4">
+        <f>F4*'Other Values'!$B$31</f>
+        <v>3.8579698245238621E-3</v>
+      </c>
+      <c r="G8" s="4">
+        <f>G4*'Other Values'!$B$31</f>
+        <v>3.8579698245238621E-3</v>
+      </c>
+      <c r="H8" s="4">
+        <f>H4*'Other Values'!$B$31</f>
+        <v>3.8579698245238621E-3</v>
+      </c>
+      <c r="I8" s="4">
+        <f>I4*'Other Values'!$B$31</f>
+        <v>3.8579698245238621E-3</v>
+      </c>
+      <c r="J8" s="4">
+        <f>J4*'Other Values'!$B$31</f>
+        <v>3.8579698245238621E-3</v>
+      </c>
+      <c r="K8" s="4">
+        <f>K4*'Other Values'!$B$31</f>
+        <v>3.8579698245238621E-3</v>
+      </c>
+      <c r="L8" s="4">
+        <f>L4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="M8" s="4">
+        <f>M4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="N8" s="4">
+        <f>N4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="O8" s="4">
+        <f>O4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="P8" s="4">
+        <f>P4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="Q8" s="4">
+        <f>Q4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="R8" s="4">
+        <f>R4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="S8" s="4">
+        <f>S4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="T8" s="4">
+        <f>T4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="U8" s="4">
+        <f>U4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="V8" s="4">
+        <f>V4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="W8" s="4">
+        <f>W4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="X8" s="4">
+        <f>X4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="Y8" s="4">
+        <f>Y4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="Z8" s="4">
+        <f>Z4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="AA8" s="4">
+        <f>AA4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="AB8" s="4">
+        <f>AB4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="AC8" s="4">
+        <f>AC4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="AD8" s="4">
+        <f>AD4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="AE8" s="4">
+        <f>AE4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="AF8" s="4">
+        <f>AF4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="AG8" s="4">
+        <f>AG4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="AH8" s="4">
+        <f>AH4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
+      </c>
+      <c r="AI8" s="4">
+        <f>AI4*'Other Values'!$B$31</f>
+        <v>3.8579698245238643E-3</v>
       </c>
     </row>
     <row r="13" spans="1:35">
@@ -11440,7 +11530,7 @@
   <dimension ref="A1:AI8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:AI8"/>
+      <selection activeCell="B8" sqref="B8:AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -12405,107 +12495,141 @@
       <c r="A8" t="s">
         <v>55</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
-      </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <v>0</v>
-      </c>
-      <c r="AD8">
-        <v>0</v>
-      </c>
-      <c r="AE8">
-        <v>0</v>
-      </c>
-      <c r="AF8">
-        <v>0</v>
-      </c>
-      <c r="AG8">
-        <v>0</v>
-      </c>
-      <c r="AH8">
-        <v>0</v>
-      </c>
-      <c r="AI8">
-        <v>0</v>
+      <c r="B8" s="4">
+        <f>B4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="C8" s="4">
+        <f>C4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="D8" s="4">
+        <f>D4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="E8" s="4">
+        <f>E4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="F8" s="4">
+        <f>F4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="G8" s="4">
+        <f>G4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="H8" s="4">
+        <f>H4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="I8" s="4">
+        <f>I4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="J8" s="4">
+        <f>J4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="K8" s="4">
+        <f>K4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="L8" s="4">
+        <f>L4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="M8" s="4">
+        <f>M4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="N8" s="4">
+        <f>N4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="O8" s="4">
+        <f>O4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="P8" s="4">
+        <f>P4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="Q8" s="4">
+        <f>Q4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="R8" s="4">
+        <f>R4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="S8" s="4">
+        <f>S4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="T8" s="4">
+        <f>T4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="U8" s="4">
+        <f>U4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="V8" s="4">
+        <f>V4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="W8" s="4">
+        <f>W4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="X8" s="4">
+        <f>X4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="Y8" s="4">
+        <f>Y4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="Z8" s="4">
+        <f>Z4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="AA8" s="4">
+        <f>AA4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="AB8" s="4">
+        <f>AB4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="AC8" s="4">
+        <f>AC4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="AD8" s="4">
+        <f>AD4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="AE8" s="4">
+        <f>AE4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="AF8" s="4">
+        <f>AF4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="AG8" s="4">
+        <f>AG4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="AH8" s="4">
+        <f>AH4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
+      </c>
+      <c r="AI8" s="4">
+        <f>AI4*'Other Values'!$B$31</f>
+        <v>2.9708482131547745E-3</v>
       </c>
     </row>
   </sheetData>
@@ -12517,7 +12641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK19"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="D15" sqref="D15:AK15"/>
     </sheetView>
   </sheetViews>
@@ -14064,10 +14188,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -14383,6 +14507,37 @@
     <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31">
+        <f>B30/B29</f>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -17987,8 +18142,8 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -18953,107 +19108,141 @@
       <c r="A8" t="s">
         <v>55</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
-      </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <v>0</v>
-      </c>
-      <c r="AD8">
-        <v>0</v>
-      </c>
-      <c r="AE8">
-        <v>0</v>
-      </c>
-      <c r="AF8">
-        <v>0</v>
-      </c>
-      <c r="AG8">
-        <v>0</v>
-      </c>
-      <c r="AH8">
-        <v>0</v>
-      </c>
-      <c r="AI8">
-        <v>0</v>
+      <c r="B8" s="4">
+        <f>B4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="C8" s="4">
+        <f>C4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="D8" s="4">
+        <f>D4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="E8" s="4">
+        <f>E4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="F8" s="4">
+        <f>F4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="G8" s="4">
+        <f>G4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="H8" s="4">
+        <f>H4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="I8" s="4">
+        <f>I4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="J8" s="4">
+        <f>J4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="K8" s="4">
+        <f>K4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="L8" s="4">
+        <f>L4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="M8" s="4">
+        <f>M4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="N8" s="4">
+        <f>N4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="O8" s="4">
+        <f>O4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="P8" s="4">
+        <f>P4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="Q8" s="4">
+        <f>Q4*'Other Values'!$B$31</f>
+        <v>1.5970611503048245E-3</v>
+      </c>
+      <c r="R8" s="4">
+        <f>R4*'Other Values'!$B$31</f>
+        <v>1.6436490670987403E-3</v>
+      </c>
+      <c r="S8" s="4">
+        <f>S4*'Other Values'!$B$31</f>
+        <v>1.6902369838926734E-3</v>
+      </c>
+      <c r="T8" s="4">
+        <f>T4*'Other Values'!$B$31</f>
+        <v>1.7368249006865892E-3</v>
+      </c>
+      <c r="U8" s="4">
+        <f>U4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="V8" s="4">
+        <f>V4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="W8" s="4">
+        <f>W4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="X8" s="4">
+        <f>X4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="Y8" s="4">
+        <f>Y4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="Z8" s="4">
+        <f>Z4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="AA8" s="4">
+        <f>AA4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="AB8" s="4">
+        <f>AB4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="AC8" s="4">
+        <f>AC4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="AD8" s="4">
+        <f>AD4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="AE8" s="4">
+        <f>AE4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="AF8" s="4">
+        <f>AF4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="AG8" s="4">
+        <f>AG4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="AH8" s="4">
+        <f>AH4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
+      </c>
+      <c r="AI8" s="4">
+        <f>AI4*'Other Values'!$B$31</f>
+        <v>1.7834128174805243E-3</v>
       </c>
     </row>
   </sheetData>
@@ -19068,8 +19257,8 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -20034,107 +20223,141 @@
       <c r="A8" t="s">
         <v>55</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8" s="8">
-        <v>0</v>
-      </c>
-      <c r="P8" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="8">
-        <v>0</v>
-      </c>
-      <c r="R8" s="8">
-        <v>0</v>
-      </c>
-      <c r="S8" s="8">
-        <v>0</v>
-      </c>
-      <c r="T8" s="8">
-        <v>0</v>
-      </c>
-      <c r="U8" s="8">
-        <v>0</v>
-      </c>
-      <c r="V8" s="8">
-        <v>0</v>
-      </c>
-      <c r="W8" s="8">
-        <v>0</v>
-      </c>
-      <c r="X8" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="8">
-        <v>0</v>
+      <c r="B8" s="4">
+        <f>B4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="C8" s="4">
+        <f>C4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="D8" s="4">
+        <f>D4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="E8" s="4">
+        <f>E4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="F8" s="4">
+        <f>F4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="G8" s="4">
+        <f>G4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="H8" s="4">
+        <f>H4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="I8" s="4">
+        <f>I4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="J8" s="4">
+        <f>J4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="K8" s="4">
+        <f>K4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="L8" s="4">
+        <f>L4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="M8" s="4">
+        <f>M4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="N8" s="4">
+        <f>N4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="O8" s="4">
+        <f>O4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="P8" s="4">
+        <f>P4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="Q8" s="4">
+        <f>Q4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="R8" s="4">
+        <f>R4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="S8" s="4">
+        <f>S4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="T8" s="4">
+        <f>T4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="U8" s="4">
+        <f>U4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="V8" s="4">
+        <f>V4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="W8" s="4">
+        <f>W4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="X8" s="4">
+        <f>X4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="Y8" s="4">
+        <f>Y4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="Z8" s="4">
+        <f>Z4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="AA8" s="4">
+        <f>AA4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="AB8" s="4">
+        <f>AB4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="AC8" s="4">
+        <f>AC4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="AD8" s="4">
+        <f>AD4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="AE8" s="4">
+        <f>AE4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="AF8" s="4">
+        <f>AF4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="AG8" s="4">
+        <f>AG4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="AH8" s="4">
+        <f>AH4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
+      </c>
+      <c r="AI8" s="4">
+        <f>AI4*'Other Values'!$B$31</f>
+        <v>8.5412569624788255E-4</v>
       </c>
     </row>
   </sheetData>
@@ -20149,8 +20372,8 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:AI7"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -21115,107 +21338,141 @@
       <c r="A8" t="s">
         <v>55</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
-      </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="8">
-        <v>0</v>
+      <c r="B8" s="4">
+        <f>B4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="C8" s="4">
+        <f>C4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="D8" s="4">
+        <f>D4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="E8" s="4">
+        <f>E4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="F8" s="4">
+        <f>F4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="G8" s="4">
+        <f>G4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="H8" s="4">
+        <f>H4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="I8" s="4">
+        <f>I4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="J8" s="4">
+        <f>J4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="K8" s="4">
+        <f>K4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="L8" s="4">
+        <f>L4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="M8" s="4">
+        <f>M4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="N8" s="4">
+        <f>N4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="O8" s="4">
+        <f>O4*'Other Values'!$B$31</f>
+        <v>1.1108892894717282E-2</v>
+      </c>
+      <c r="P8" s="4">
+        <f>P4*'Other Values'!$B$31</f>
+        <v>1.1798410384734059E-2</v>
+      </c>
+      <c r="Q8" s="4">
+        <f>Q4*'Other Values'!$B$31</f>
+        <v>1.2487927874751115E-2</v>
+      </c>
+      <c r="R8" s="4">
+        <f>R4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="S8" s="4">
+        <f>S4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="T8" s="4">
+        <f>T4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="U8" s="4">
+        <f>U4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="V8" s="4">
+        <f>V4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="W8" s="4">
+        <f>W4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="X8" s="4">
+        <f>X4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="Y8" s="4">
+        <f>Y4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="Z8" s="4">
+        <f>Z4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="AA8" s="4">
+        <f>AA4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="AB8" s="4">
+        <f>AB4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="AC8" s="4">
+        <f>AC4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="AD8" s="4">
+        <f>AD4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="AE8" s="4">
+        <f>AE4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="AF8" s="4">
+        <f>AF4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="AG8" s="4">
+        <f>AG4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="AH8" s="4">
+        <f>AH4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
+      </c>
+      <c r="AI8" s="4">
+        <f>AI4*'Other Values'!$B$31</f>
+        <v>1.3177445364767892E-2</v>
       </c>
     </row>
   </sheetData>
@@ -21231,7 +21488,7 @@
   <dimension ref="A1:AI8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:AI7"/>
+      <selection activeCell="B8" sqref="B8:AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -22196,107 +22453,141 @@
       <c r="A8" t="s">
         <v>55</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
-      </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="8">
-        <v>0</v>
+      <c r="B8" s="4">
+        <f>B4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="C8" s="4">
+        <f>C4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="D8" s="4">
+        <f>D4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="E8" s="4">
+        <f>E4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="F8" s="4">
+        <f>F4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="G8" s="4">
+        <f>G4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="H8" s="4">
+        <f>H4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="I8" s="4">
+        <f>I4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="J8" s="4">
+        <f>J4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="K8" s="4">
+        <f>K4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="L8" s="4">
+        <f>L4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="M8" s="4">
+        <f>M4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="N8" s="4">
+        <f>N4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="O8" s="4">
+        <f>O4*'Other Values'!$B$31</f>
+        <v>1.128310786557337E-3</v>
+      </c>
+      <c r="P8" s="4">
+        <f>P4*'Other Values'!$B$31</f>
+        <v>1.1907117217055396E-3</v>
+      </c>
+      <c r="Q8" s="4">
+        <f>Q4*'Other Values'!$B$31</f>
+        <v>1.2531126568537422E-3</v>
+      </c>
+      <c r="R8" s="4">
+        <f>R4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="S8" s="4">
+        <f>S4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="T8" s="4">
+        <f>T4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="U8" s="4">
+        <f>U4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="V8" s="4">
+        <f>V4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="W8" s="4">
+        <f>W4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="X8" s="4">
+        <f>X4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="Y8" s="4">
+        <f>Y4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="Z8" s="4">
+        <f>Z4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="AA8" s="4">
+        <f>AA4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="AB8" s="4">
+        <f>AB4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="AC8" s="4">
+        <f>AC4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="AD8" s="4">
+        <f>AD4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="AE8" s="4">
+        <f>AE4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="AF8" s="4">
+        <f>AF4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="AG8" s="4">
+        <f>AG4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="AH8" s="4">
+        <f>AH4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
+      </c>
+      <c r="AI8" s="4">
+        <f>AI4*'Other Values'!$B$31</f>
+        <v>1.3155135920019621E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>